<commit_message>
Fix bug in Author.js, rename Details to Order_details, add .csv files to populate the database (only events left).
</commit_message>
<xml_diff>
--- a/docs/Logical_Schema.xlsx
+++ b/docs/Logical_Schema.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Casa\Desktop\hyp-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Casa\Desktop\hyp-project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52F77DA-21BE-4704-BC83-FC292F007181}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0FE031-B5D9-4293-A361-C868749FA8A6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8100" yWindow="-80" windowWidth="14400" windowHeight="7360" xr2:uid="{F3A69DC3-4D3F-4B56-8DBC-062F1BF364F6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F3A69DC3-4D3F-4B56-8DBC-062F1BF364F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
   <si>
     <t>ISBN</t>
   </si>
@@ -147,9 +147,6 @@
     <t>rating</t>
   </si>
   <si>
-    <t>Details</t>
-  </si>
-  <si>
     <t>item_price</t>
   </si>
   <si>
@@ -169,13 +166,19 @@
   </si>
   <si>
     <t>Book_details</t>
+  </si>
+  <si>
+    <t>Order_details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All book_id fields reference book's book_id. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,6 +188,14 @@
     </font>
     <font>
       <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -282,6 +293,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1685,10 +1699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B3FF16B-F344-4345-87E1-385178718014}">
-  <dimension ref="C1:M29"/>
+  <dimension ref="C1:M31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1712,7 +1726,7 @@
     </row>
     <row r="2" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C2" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
@@ -1758,7 +1772,7 @@
     </row>
     <row r="4" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C4" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -1773,7 +1787,7 @@
     </row>
     <row r="5" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>12</v>
@@ -1874,7 +1888,7 @@
         <v>19</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>20</v>
@@ -1979,7 +1993,7 @@
         <v>30</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>31</v>
@@ -1988,7 +2002,7 @@
         <v>32</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
@@ -2007,7 +2021,7 @@
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
+      <c r="M18" s="9"/>
     </row>
     <row r="19" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C19" s="4" t="s">
@@ -2029,7 +2043,7 @@
         <v>15</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>12</v>
@@ -2078,7 +2092,7 @@
         <v>15</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>36</v>
@@ -2087,7 +2101,7 @@
         <v>37</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
@@ -2111,7 +2125,7 @@
     </row>
     <row r="25" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C25" s="4" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -2129,13 +2143,13 @@
         <v>19</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>34</v>
@@ -2162,7 +2176,7 @@
     </row>
     <row r="28" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C28" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
@@ -2180,7 +2194,7 @@
         <v>24</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
@@ -2192,6 +2206,11 @@
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
     </row>
+    <row r="31" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C31" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>